<commit_message>
update police avoidance to fix typo
</commit_message>
<xml_diff>
--- a/police_avoidance.xlsx
+++ b/police_avoidance.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryantracy/Desktop/andre rc studies/police meta perceptions project/study 1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryantracy/Desktop/andre rc studies/police meta perceptions project/study 2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{322A5386-433E-FE42-ACF5-F49126A24B1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B7AD753-7863-DC42-8808-C0549F0F3701}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3660" yWindow="2660" windowWidth="27640" windowHeight="16940" xr2:uid="{735FF316-57A2-AB45-8D69-C51B7A751742}"/>
   </bookViews>
@@ -59,9 +59,6 @@
     <t>police_avoidance3</t>
   </si>
   <si>
-    <t>Plan drive/walk How often do you plan where to drive/ walk to make sure that you do not attract attention from the police?</t>
-  </si>
-  <si>
     <t>police_avoidance4</t>
   </si>
   <si>
@@ -93,6 +90,9 @@
   </si>
   <si>
     <t>How often do you have contact with the police  in your daily life (e.g., seeing, speaking to, or interacting with them)?</t>
+  </si>
+  <si>
+    <t>How often do you plan where to drive/ walk to make sure that you do not attract attention from the police?</t>
   </si>
 </sst>
 </file>
@@ -467,7 +467,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -478,16 +478,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
         <v>14</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>15</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>16</v>
-      </c>
-      <c r="D1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -523,7 +523,7 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="C4" t="s">
         <v>2</v>
@@ -534,10 +534,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
         <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
       </c>
       <c r="C5" t="s">
         <v>2</v>
@@ -548,10 +548,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
         <v>10</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
       </c>
       <c r="C6" t="s">
         <v>2</v>
@@ -562,16 +562,16 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C7" t="s">
         <v>2</v>
       </c>
       <c r="D7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>